<commit_message>
Added promo models / initial sql scripts
</commit_message>
<xml_diff>
--- a/Backend/group3site/jeans/generatedfiles/DataDict.xlsx
+++ b/Backend/group3site/jeans/generatedfiles/DataDict.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="61">
   <si>
     <t>Load Order</t>
   </si>
@@ -61,36 +61,48 @@
     <t>Table Desc</t>
   </si>
   <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>Standard Auto-Increment PK</t>
+  </si>
+  <si>
+    <t>A link to an image</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>image_url</t>
+  </si>
+  <si>
+    <t>nvarchar</t>
+  </si>
+  <si>
+    <t>image_caption</t>
+  </si>
+  <si>
     <t>ProductStatus</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>UNIQUE</t>
-  </si>
-  <si>
-    <t>Standard Auto-Increment PK</t>
-  </si>
-  <si>
     <t>Refers to the current state of the product</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>status_name</t>
   </si>
   <si>
-    <t>nvarchar</t>
-  </si>
-  <si>
     <t>status_desc</t>
   </si>
   <si>
@@ -121,9 +133,6 @@
     <t>brand_site</t>
   </si>
   <si>
-    <t>URLField</t>
-  </si>
-  <si>
     <t>Product</t>
   </si>
   <si>
@@ -148,10 +157,16 @@
     <t>product_brand_id</t>
   </si>
   <si>
-    <t>product_tags</t>
-  </si>
-  <si>
-    <t>ManyToManyField</t>
+    <t>Promo</t>
+  </si>
+  <si>
+    <t>Describes a promotion for a group of products</t>
+  </si>
+  <si>
+    <t>promo_name</t>
+  </si>
+  <si>
+    <t>promo_code</t>
   </si>
   <si>
     <t>ProductProductTag</t>
@@ -164,6 +179,24 @@
   </si>
   <si>
     <t>product_tag_id</t>
+  </si>
+  <si>
+    <t>ProductImage</t>
+  </si>
+  <si>
+    <t>Used to associate an Image with a Product</t>
+  </si>
+  <si>
+    <t>product_image_id</t>
+  </si>
+  <si>
+    <t>ProductPromo</t>
+  </si>
+  <si>
+    <t>Used to associate a Product with a Promo</t>
+  </si>
+  <si>
+    <t>promo_id</t>
   </si>
 </sst>
 </file>
@@ -211,8 +244,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O31" totalsRowShown="0">
-  <autoFilter ref="A1:O31"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O43" totalsRowShown="0">
+  <autoFilter ref="A1:O43"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Load Order"/>
     <tableColumn id="2" name="Table Name"/>
@@ -519,7 +552,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -530,7 +563,7 @@
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="8" width="7" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" customWidth="1"/>
@@ -648,7 +681,7 @@
         <v>17</v>
       </c>
       <c r="E3">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -722,71 +755,74 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
+    <row r="6" spans="1:15">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" t="s">
         <v>27</v>
       </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="b">
-        <v>0</v>
-      </c>
-      <c r="K5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" t="b">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7">
-        <v>1</v>
+      <c r="A7" t="s">
+        <v>22</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="s">
-        <v>17</v>
+      <c r="E7">
+        <v>40</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -804,13 +840,10 @@
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -821,13 +854,13 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
       </c>
       <c r="E8">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
@@ -839,10 +872,10 @@
         <v>0</v>
       </c>
       <c r="I8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" t="b">
         <v>0</v>
@@ -865,107 +898,110 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9">
-        <v>200</v>
+        <v>30</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
       </c>
       <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>0</v>
+      </c>
+      <c r="L11" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
         <v>24</v>
       </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" t="b">
-        <v>0</v>
-      </c>
-      <c r="M9" t="s">
-        <v>17</v>
-      </c>
-      <c r="O9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" t="b">
-        <v>0</v>
-      </c>
-      <c r="K10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" t="b">
-        <v>0</v>
-      </c>
-      <c r="M10" t="s">
-        <v>17</v>
-      </c>
-      <c r="O10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
       <c r="G12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -983,13 +1019,10 @@
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>19</v>
-      </c>
-      <c r="N12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O12" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1000,13 +1033,13 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
       </c>
       <c r="E13">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="F13" t="s">
         <v>24</v>
@@ -1018,10 +1051,10 @@
         <v>0</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" t="b">
         <v>0</v>
@@ -1044,107 +1077,110 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14">
-        <v>200</v>
+        <v>30</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
       </c>
       <c r="F14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G14" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>80</v>
+      </c>
+      <c r="F17" t="s">
         <v>24</v>
       </c>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" t="b">
-        <v>0</v>
-      </c>
-      <c r="M14" t="s">
-        <v>17</v>
-      </c>
-      <c r="O14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15">
-        <v>200</v>
-      </c>
-      <c r="F15" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" t="b">
-        <v>0</v>
-      </c>
-      <c r="M15" t="s">
-        <v>17</v>
-      </c>
-      <c r="O15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
       <c r="G17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
@@ -1162,13 +1198,10 @@
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>19</v>
-      </c>
-      <c r="N17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O17" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1179,13 +1212,13 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
       </c>
       <c r="E18">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
@@ -1197,10 +1230,10 @@
         <v>0</v>
       </c>
       <c r="I18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" t="b">
         <v>0</v>
@@ -1223,7 +1256,7 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
@@ -1241,10 +1274,10 @@
         <v>0</v>
       </c>
       <c r="I19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" t="b">
         <v>0</v>
@@ -1259,59 +1292,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>19</v>
-      </c>
-      <c r="F20" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" t="b">
-        <v>0</v>
-      </c>
-      <c r="K20" t="b">
-        <v>0</v>
-      </c>
-      <c r="L20" t="b">
-        <v>0</v>
-      </c>
-      <c r="M20" t="s">
-        <v>42</v>
-      </c>
-      <c r="O20" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="21" spans="1:15">
-      <c r="A21" t="s">
-        <v>22</v>
+      <c r="A21">
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
@@ -1323,10 +1312,10 @@
         <v>18</v>
       </c>
       <c r="G21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
@@ -1341,10 +1330,13 @@
         <v>0</v>
       </c>
       <c r="M21" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="N21" t="s">
+        <v>20</v>
       </c>
       <c r="O21" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1355,87 +1347,128 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22">
+        <v>80</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" t="b">
+        <v>0</v>
+      </c>
+      <c r="M22" t="s">
+        <v>17</v>
+      </c>
+      <c r="O22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <v>200</v>
+      </c>
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23" t="b">
+        <v>0</v>
+      </c>
+      <c r="M23" t="s">
+        <v>17</v>
+      </c>
+      <c r="O23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
         <v>44</v>
       </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" t="b">
+        <v>0</v>
+      </c>
+      <c r="M24" t="s">
         <v>45</v>
       </c>
-      <c r="G22" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" t="b">
-        <v>0</v>
-      </c>
-      <c r="K22" t="b">
-        <v>0</v>
-      </c>
-      <c r="L22" t="b">
-        <v>0</v>
-      </c>
-      <c r="M22" t="s">
-        <v>17</v>
-      </c>
-      <c r="O22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" t="b">
-        <v>1</v>
-      </c>
-      <c r="H24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" t="b">
-        <v>0</v>
-      </c>
-      <c r="K24" t="b">
-        <v>0</v>
-      </c>
-      <c r="L24" t="b">
-        <v>0</v>
-      </c>
-      <c r="M24" t="s">
-        <v>19</v>
-      </c>
-      <c r="N24" t="s">
-        <v>20</v>
-      </c>
       <c r="O24" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1446,22 +1479,22 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
       </c>
-      <c r="E25">
-        <v>40</v>
+      <c r="E25" t="s">
+        <v>17</v>
       </c>
       <c r="F25" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
       </c>
       <c r="H25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -1482,71 +1515,27 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
-        <v>17</v>
-      </c>
-      <c r="E26">
-        <v>200</v>
-      </c>
-      <c r="F26" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" t="b">
-        <v>0</v>
-      </c>
-      <c r="J26" t="b">
-        <v>1</v>
-      </c>
-      <c r="K26" t="b">
-        <v>0</v>
-      </c>
-      <c r="L26" t="b">
-        <v>0</v>
-      </c>
-      <c r="M26" t="s">
-        <v>17</v>
-      </c>
-      <c r="O26" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="27" spans="1:15">
-      <c r="A27" t="s">
-        <v>22</v>
+      <c r="A27">
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" t="b">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
       </c>
       <c r="E27" t="s">
         <v>17</v>
       </c>
       <c r="F27" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -1564,10 +1553,13 @@
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="N27" t="s">
+        <v>20</v>
       </c>
       <c r="O27" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -1578,22 +1570,22 @@
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
       </c>
-      <c r="E28" t="s">
-        <v>17</v>
+      <c r="E28">
+        <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G28" t="b">
         <v>0</v>
       </c>
       <c r="H28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -1622,39 +1614,444 @@
         <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
       </c>
-      <c r="E29" t="s">
-        <v>17</v>
+      <c r="E29">
+        <v>10</v>
       </c>
       <c r="F29" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" t="b">
+        <v>0</v>
+      </c>
+      <c r="L29" t="b">
+        <v>0</v>
+      </c>
+      <c r="M29" t="s">
+        <v>17</v>
+      </c>
+      <c r="O29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" t="s">
         <v>18</v>
       </c>
-      <c r="G29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" t="b">
-        <v>0</v>
-      </c>
-      <c r="K29" t="b">
-        <v>0</v>
-      </c>
-      <c r="L29" t="b">
-        <v>0</v>
-      </c>
-      <c r="M29" t="s">
-        <v>17</v>
-      </c>
-      <c r="O29" t="s">
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" t="b">
+        <v>0</v>
+      </c>
+      <c r="L31" t="b">
+        <v>0</v>
+      </c>
+      <c r="M31" t="s">
+        <v>19</v>
+      </c>
+      <c r="N31" t="s">
+        <v>20</v>
+      </c>
+      <c r="O31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <v>0</v>
+      </c>
+      <c r="L32" t="b">
+        <v>0</v>
+      </c>
+      <c r="M32" t="s">
+        <v>17</v>
+      </c>
+      <c r="O32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="b">
+        <v>0</v>
+      </c>
+      <c r="L33" t="b">
+        <v>0</v>
+      </c>
+      <c r="M33" t="s">
+        <v>17</v>
+      </c>
+      <c r="O33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" t="b">
+        <v>0</v>
+      </c>
+      <c r="L35" t="b">
+        <v>0</v>
+      </c>
+      <c r="M35" t="s">
+        <v>19</v>
+      </c>
+      <c r="N35" t="s">
+        <v>20</v>
+      </c>
+      <c r="O35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" t="b">
+        <v>0</v>
+      </c>
+      <c r="L36" t="b">
+        <v>0</v>
+      </c>
+      <c r="M36" t="s">
+        <v>17</v>
+      </c>
+      <c r="O36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" t="b">
+        <v>0</v>
+      </c>
+      <c r="L37" t="b">
+        <v>0</v>
+      </c>
+      <c r="M37" t="s">
+        <v>17</v>
+      </c>
+      <c r="O37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="b">
+        <v>0</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" t="b">
+        <v>0</v>
+      </c>
+      <c r="L39" t="b">
+        <v>0</v>
+      </c>
+      <c r="M39" t="s">
+        <v>19</v>
+      </c>
+      <c r="N39" t="s">
+        <v>20</v>
+      </c>
+      <c r="O39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" t="b">
+        <v>0</v>
+      </c>
+      <c r="L40" t="b">
+        <v>0</v>
+      </c>
+      <c r="M40" t="s">
+        <v>17</v>
+      </c>
+      <c r="O40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" t="b">
+        <v>0</v>
+      </c>
+      <c r="L41" t="b">
+        <v>0</v>
+      </c>
+      <c r="M41" t="s">
+        <v>17</v>
+      </c>
+      <c r="O41" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added nav buttons/listview/simple forms
</commit_message>
<xml_diff>
--- a/Backend/group3site/jeans/generatedfiles/DataDict.xlsx
+++ b/Backend/group3site/jeans/generatedfiles/DataDict.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="66">
   <si>
     <t>Load Order</t>
   </si>
@@ -197,6 +197,21 @@
   </si>
   <si>
     <t>promo_id</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Name and email for a customer who will recieve promo emails</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -244,8 +259,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O43" totalsRowShown="0">
-  <autoFilter ref="A1:O43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O48" totalsRowShown="0">
+  <autoFilter ref="A1:O48"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Load Order"/>
     <tableColumn id="2" name="Table Name"/>
@@ -552,7 +567,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -570,7 +585,7 @@
     <col min="11" max="12" width="10.7109375" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" customWidth="1"/>
     <col min="14" max="14" width="33.28515625" customWidth="1"/>
-    <col min="15" max="15" width="57" customWidth="1"/>
+    <col min="15" max="15" width="74.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -1644,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="M29" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O29" t="s">
         <v>22</v>
@@ -2052,6 +2067,185 @@
         <v>17</v>
       </c>
       <c r="O41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" t="b">
+        <v>0</v>
+      </c>
+      <c r="L43" t="b">
+        <v>0</v>
+      </c>
+      <c r="M43" t="s">
+        <v>19</v>
+      </c>
+      <c r="N43" t="s">
+        <v>20</v>
+      </c>
+      <c r="O43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" t="s">
+        <v>17</v>
+      </c>
+      <c r="E44">
+        <v>200</v>
+      </c>
+      <c r="F44" t="s">
+        <v>24</v>
+      </c>
+      <c r="G44" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" t="b">
+        <v>0</v>
+      </c>
+      <c r="L44" t="b">
+        <v>0</v>
+      </c>
+      <c r="M44" t="s">
+        <v>17</v>
+      </c>
+      <c r="O44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45">
+        <v>200</v>
+      </c>
+      <c r="F45" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+      <c r="J45" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" t="b">
+        <v>0</v>
+      </c>
+      <c r="L45" t="b">
+        <v>0</v>
+      </c>
+      <c r="M45" t="s">
+        <v>17</v>
+      </c>
+      <c r="O45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46">
+        <v>254</v>
+      </c>
+      <c r="F46" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" t="b">
+        <v>0</v>
+      </c>
+      <c r="L46" t="b">
+        <v>0</v>
+      </c>
+      <c r="M46" t="s">
+        <v>17</v>
+      </c>
+      <c r="O46" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added date fields and Promo Status
</commit_message>
<xml_diff>
--- a/Backend/group3site/jeans/generatedfiles/DataDict.xlsx
+++ b/Backend/group3site/jeans/generatedfiles/DataDict.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="72">
   <si>
     <t>Load Order</t>
   </si>
@@ -112,6 +112,12 @@
     <t>bit</t>
   </si>
   <si>
+    <t>PromoStatus</t>
+  </si>
+  <si>
+    <t>Refers to the current state of the promo</t>
+  </si>
+  <si>
     <t>ProductTag</t>
   </si>
   <si>
@@ -157,6 +163,15 @@
     <t>product_brand_id</t>
   </si>
   <si>
+    <t>product_status_id</t>
+  </si>
+  <si>
+    <t>created_date</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
     <t>Promo</t>
   </si>
   <si>
@@ -167,6 +182,9 @@
   </si>
   <si>
     <t>promo_code</t>
+  </si>
+  <si>
+    <t>promo_status_id</t>
   </si>
   <si>
     <t>ProductProductTag</t>
@@ -259,8 +277,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O48" totalsRowShown="0">
-  <autoFilter ref="A1:O48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O59" totalsRowShown="0">
+  <autoFilter ref="A1:O59"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Load Order"/>
     <tableColumn id="2" name="Table Name"/>
@@ -567,15 +585,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
@@ -1183,13 +1200,13 @@
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
       </c>
       <c r="E17">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s">
         <v>24</v>
@@ -1227,7 +1244,7 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
@@ -1271,16 +1288,16 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19">
-        <v>200</v>
+        <v>30</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="G19" t="b">
         <v>0</v>
@@ -1309,10 +1326,10 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
@@ -1351,7 +1368,7 @@
         <v>20</v>
       </c>
       <c r="O21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1362,7 +1379,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -1406,7 +1423,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -1450,107 +1467,110 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24">
+        <v>200</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" t="b">
+        <v>0</v>
+      </c>
+      <c r="M24" t="s">
+        <v>17</v>
+      </c>
+      <c r="O24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26" t="b">
+        <v>0</v>
+      </c>
+      <c r="M26" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" t="s">
+        <v>20</v>
+      </c>
+      <c r="O26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
         <v>43</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>19</v>
-      </c>
-      <c r="F24" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" t="b">
-        <v>0</v>
-      </c>
-      <c r="K24" t="b">
-        <v>0</v>
-      </c>
-      <c r="L24" t="b">
-        <v>0</v>
-      </c>
-      <c r="M24" t="s">
-        <v>45</v>
-      </c>
-      <c r="O24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25" t="b">
-        <v>0</v>
-      </c>
-      <c r="K25" t="b">
-        <v>0</v>
-      </c>
-      <c r="L25" t="b">
-        <v>0</v>
-      </c>
-      <c r="M25" t="s">
-        <v>17</v>
-      </c>
-      <c r="O25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27">
-        <v>2</v>
-      </c>
-      <c r="B27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
       <c r="D27" t="s">
         <v>17</v>
       </c>
-      <c r="E27" t="s">
-        <v>17</v>
+      <c r="E27">
+        <v>80</v>
       </c>
       <c r="F27" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" t="b">
         <v>0</v>
@@ -1568,13 +1588,10 @@
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>19</v>
-      </c>
-      <c r="N27" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O27" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -1585,13 +1602,13 @@
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
       </c>
       <c r="E28">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="F28" t="s">
         <v>24</v>
@@ -1603,10 +1620,10 @@
         <v>0</v>
       </c>
       <c r="I28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" t="b">
         <v>0</v>
@@ -1629,16 +1646,16 @@
         <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>17</v>
+        <v>45</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F29" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="G29" t="b">
         <v>0</v>
@@ -1659,21 +1676,65 @@
         <v>0</v>
       </c>
       <c r="M29" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="O29" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="30" spans="1:15">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L30" t="b">
+        <v>0</v>
+      </c>
+      <c r="M30" t="s">
+        <v>17</v>
+      </c>
+      <c r="O30" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="31" spans="1:15">
-      <c r="A31">
-        <v>3</v>
+      <c r="A31" t="s">
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -1685,10 +1746,10 @@
         <v>18</v>
       </c>
       <c r="G31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
@@ -1703,13 +1764,10 @@
         <v>0</v>
       </c>
       <c r="M31" t="s">
-        <v>19</v>
-      </c>
-      <c r="N31" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O31" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -1720,107 +1778,110 @@
         <v>22</v>
       </c>
       <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" t="b">
+        <v>0</v>
+      </c>
+      <c r="L32" t="b">
+        <v>0</v>
+      </c>
+      <c r="M32" t="s">
+        <v>17</v>
+      </c>
+      <c r="O32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" t="b">
+        <v>0</v>
+      </c>
+      <c r="L34" t="b">
+        <v>0</v>
+      </c>
+      <c r="M34" t="s">
+        <v>19</v>
+      </c>
+      <c r="N34" t="s">
+        <v>20</v>
+      </c>
+      <c r="O34" t="s">
         <v>53</v>
       </c>
-      <c r="D32" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" t="s">
-        <v>17</v>
-      </c>
-      <c r="F32" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" t="b">
-        <v>1</v>
-      </c>
-      <c r="J32" t="b">
-        <v>0</v>
-      </c>
-      <c r="K32" t="b">
-        <v>0</v>
-      </c>
-      <c r="L32" t="b">
-        <v>0</v>
-      </c>
-      <c r="M32" t="s">
-        <v>17</v>
-      </c>
-      <c r="O32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" t="s">
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" t="s">
         <v>54</v>
       </c>
-      <c r="D33" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33" t="b">
-        <v>1</v>
-      </c>
-      <c r="J33" t="b">
-        <v>0</v>
-      </c>
-      <c r="K33" t="b">
-        <v>0</v>
-      </c>
-      <c r="L33" t="b">
-        <v>0</v>
-      </c>
-      <c r="M33" t="s">
-        <v>17</v>
-      </c>
-      <c r="O33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35">
-        <v>3</v>
-      </c>
-      <c r="B35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" t="s">
-        <v>16</v>
-      </c>
       <c r="D35" t="s">
         <v>17</v>
       </c>
-      <c r="E35" t="s">
-        <v>17</v>
+      <c r="E35">
+        <v>80</v>
       </c>
       <c r="F35" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -1838,13 +1899,10 @@
         <v>0</v>
       </c>
       <c r="M35" t="s">
-        <v>19</v>
-      </c>
-      <c r="N35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="O35" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -1855,22 +1913,22 @@
         <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
         <v>17</v>
       </c>
-      <c r="E36" t="s">
-        <v>17</v>
+      <c r="E36">
+        <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G36" t="b">
         <v>0</v>
       </c>
       <c r="H36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
@@ -1885,7 +1943,7 @@
         <v>0</v>
       </c>
       <c r="M36" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O36" t="s">
         <v>22</v>
@@ -1899,7 +1957,7 @@
         <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
@@ -1935,62 +1993,59 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
-      <c r="A39">
+    <row r="38" spans="1:15">
+      <c r="A38" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" t="b">
+        <v>0</v>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" t="b">
+        <v>0</v>
+      </c>
+      <c r="L38" t="b">
+        <v>0</v>
+      </c>
+      <c r="M38" t="s">
+        <v>17</v>
+      </c>
+      <c r="O38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="A40">
         <v>3</v>
       </c>
-      <c r="B39" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" t="s">
         <v>16</v>
-      </c>
-      <c r="D39" t="s">
-        <v>17</v>
-      </c>
-      <c r="E39" t="s">
-        <v>17</v>
-      </c>
-      <c r="F39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" t="b">
-        <v>0</v>
-      </c>
-      <c r="I39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J39" t="b">
-        <v>0</v>
-      </c>
-      <c r="K39" t="b">
-        <v>0</v>
-      </c>
-      <c r="L39" t="b">
-        <v>0</v>
-      </c>
-      <c r="M39" t="s">
-        <v>19</v>
-      </c>
-      <c r="N39" t="s">
-        <v>20</v>
-      </c>
-      <c r="O39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="A40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" t="s">
-        <v>53</v>
       </c>
       <c r="D40" t="s">
         <v>17</v>
@@ -2002,10 +2057,10 @@
         <v>18</v>
       </c>
       <c r="G40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
@@ -2020,10 +2075,13 @@
         <v>0</v>
       </c>
       <c r="M40" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="N40" t="s">
+        <v>20</v>
       </c>
       <c r="O40" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:15">
@@ -2034,7 +2092,7 @@
         <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D41" t="s">
         <v>17</v>
@@ -2070,139 +2128,139 @@
         <v>22</v>
       </c>
     </row>
+    <row r="42" spans="1:15">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" t="b">
+        <v>0</v>
+      </c>
+      <c r="L42" t="b">
+        <v>0</v>
+      </c>
+      <c r="M42" t="s">
+        <v>17</v>
+      </c>
+      <c r="O42" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="43" spans="1:15">
-      <c r="A43">
-        <v>1</v>
+      <c r="A43" t="s">
+        <v>22</v>
       </c>
       <c r="B43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" t="s">
+        <v>51</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" t="b">
+        <v>0</v>
+      </c>
+      <c r="L43" t="b">
+        <v>0</v>
+      </c>
+      <c r="M43" t="s">
+        <v>17</v>
+      </c>
+      <c r="O43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
         <v>61</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C45" t="s">
         <v>16</v>
       </c>
-      <c r="D43" t="s">
-        <v>17</v>
-      </c>
-      <c r="E43" t="s">
-        <v>17</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="D45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" t="s">
         <v>18</v>
       </c>
-      <c r="G43" t="b">
-        <v>1</v>
-      </c>
-      <c r="H43" t="b">
-        <v>0</v>
-      </c>
-      <c r="I43" t="b">
-        <v>1</v>
-      </c>
-      <c r="J43" t="b">
-        <v>0</v>
-      </c>
-      <c r="K43" t="b">
-        <v>0</v>
-      </c>
-      <c r="L43" t="b">
-        <v>0</v>
-      </c>
-      <c r="M43" t="s">
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+      <c r="J45" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" t="b">
+        <v>0</v>
+      </c>
+      <c r="L45" t="b">
+        <v>0</v>
+      </c>
+      <c r="M45" t="s">
         <v>19</v>
       </c>
-      <c r="N43" t="s">
+      <c r="N45" t="s">
         <v>20</v>
       </c>
-      <c r="O43" t="s">
+      <c r="O45" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15">
-      <c r="A44" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" t="s">
-        <v>17</v>
-      </c>
-      <c r="E44">
-        <v>200</v>
-      </c>
-      <c r="F44" t="s">
-        <v>24</v>
-      </c>
-      <c r="G44" t="b">
-        <v>0</v>
-      </c>
-      <c r="H44" t="b">
-        <v>0</v>
-      </c>
-      <c r="I44" t="b">
-        <v>1</v>
-      </c>
-      <c r="J44" t="b">
-        <v>0</v>
-      </c>
-      <c r="K44" t="b">
-        <v>0</v>
-      </c>
-      <c r="L44" t="b">
-        <v>0</v>
-      </c>
-      <c r="M44" t="s">
-        <v>17</v>
-      </c>
-      <c r="O44" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="A45" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45">
-        <v>200</v>
-      </c>
-      <c r="F45" t="s">
-        <v>24</v>
-      </c>
-      <c r="G45" t="b">
-        <v>0</v>
-      </c>
-      <c r="H45" t="b">
-        <v>0</v>
-      </c>
-      <c r="I45" t="b">
-        <v>1</v>
-      </c>
-      <c r="J45" t="b">
-        <v>0</v>
-      </c>
-      <c r="K45" t="b">
-        <v>0</v>
-      </c>
-      <c r="L45" t="b">
-        <v>0</v>
-      </c>
-      <c r="M45" t="s">
-        <v>17</v>
-      </c>
-      <c r="O45" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -2213,39 +2271,441 @@
         <v>22</v>
       </c>
       <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" t="s">
+        <v>17</v>
+      </c>
+      <c r="F46" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" t="b">
+        <v>0</v>
+      </c>
+      <c r="L46" t="b">
+        <v>0</v>
+      </c>
+      <c r="M46" t="s">
+        <v>17</v>
+      </c>
+      <c r="O46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F47" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" t="b">
+        <v>0</v>
+      </c>
+      <c r="L47" t="b">
+        <v>0</v>
+      </c>
+      <c r="M47" t="s">
+        <v>17</v>
+      </c>
+      <c r="O47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" t="s">
+        <v>17</v>
+      </c>
+      <c r="E49" t="s">
+        <v>17</v>
+      </c>
+      <c r="F49" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
+      <c r="J49" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" t="b">
+        <v>0</v>
+      </c>
+      <c r="L49" t="b">
+        <v>0</v>
+      </c>
+      <c r="M49" t="s">
+        <v>19</v>
+      </c>
+      <c r="N49" t="s">
+        <v>20</v>
+      </c>
+      <c r="O49" t="s">
         <v>65</v>
       </c>
-      <c r="D46" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46">
+    </row>
+    <row r="50" spans="1:15">
+      <c r="A50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" t="s">
+        <v>59</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" t="s">
+        <v>17</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+      <c r="J50" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" t="b">
+        <v>0</v>
+      </c>
+      <c r="L50" t="b">
+        <v>0</v>
+      </c>
+      <c r="M50" t="s">
+        <v>17</v>
+      </c>
+      <c r="O50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
+      <c r="A51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" t="b">
+        <v>0</v>
+      </c>
+      <c r="L51" t="b">
+        <v>0</v>
+      </c>
+      <c r="M51" t="s">
+        <v>17</v>
+      </c>
+      <c r="O51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" t="b">
+        <v>1</v>
+      </c>
+      <c r="J53" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" t="b">
+        <v>0</v>
+      </c>
+      <c r="L53" t="b">
+        <v>0</v>
+      </c>
+      <c r="M53" t="s">
+        <v>19</v>
+      </c>
+      <c r="N53" t="s">
+        <v>20</v>
+      </c>
+      <c r="O53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54">
+        <v>200</v>
+      </c>
+      <c r="F54" t="s">
+        <v>24</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" t="b">
+        <v>1</v>
+      </c>
+      <c r="J54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" t="b">
+        <v>0</v>
+      </c>
+      <c r="L54" t="b">
+        <v>0</v>
+      </c>
+      <c r="M54" t="s">
+        <v>17</v>
+      </c>
+      <c r="O54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55">
+        <v>200</v>
+      </c>
+      <c r="F55" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" t="b">
+        <v>1</v>
+      </c>
+      <c r="J55" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" t="b">
+        <v>0</v>
+      </c>
+      <c r="L55" t="b">
+        <v>0</v>
+      </c>
+      <c r="M55" t="s">
+        <v>17</v>
+      </c>
+      <c r="O55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56">
         <v>254</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F56" t="s">
         <v>24</v>
       </c>
-      <c r="G46" t="b">
-        <v>0</v>
-      </c>
-      <c r="H46" t="b">
-        <v>0</v>
-      </c>
-      <c r="I46" t="b">
-        <v>1</v>
-      </c>
-      <c r="J46" t="b">
-        <v>0</v>
-      </c>
-      <c r="K46" t="b">
-        <v>0</v>
-      </c>
-      <c r="L46" t="b">
-        <v>0</v>
-      </c>
-      <c r="M46" t="s">
-        <v>17</v>
-      </c>
-      <c r="O46" t="s">
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="b">
+        <v>1</v>
+      </c>
+      <c r="J56" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" t="b">
+        <v>0</v>
+      </c>
+      <c r="L56" t="b">
+        <v>0</v>
+      </c>
+      <c r="M56" t="s">
+        <v>17</v>
+      </c>
+      <c r="O56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" t="s">
+        <v>50</v>
+      </c>
+      <c r="D57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" t="s">
+        <v>51</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" t="b">
+        <v>1</v>
+      </c>
+      <c r="J57" t="b">
+        <v>0</v>
+      </c>
+      <c r="K57" t="b">
+        <v>0</v>
+      </c>
+      <c r="L57" t="b">
+        <v>0</v>
+      </c>
+      <c r="M57" t="s">
+        <v>17</v>
+      </c>
+      <c r="O57" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Better Money Support / Moved CustomerPromoForm into Customer Form
</commit_message>
<xml_diff>
--- a/Backend/group3site/jeans/generatedfiles/DataDict.xlsx
+++ b/Backend/group3site/jeans/generatedfiles/DataDict.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="83">
   <si>
     <t>Load Order</t>
   </si>
@@ -151,6 +151,12 @@
     <t>product_desc</t>
   </si>
   <si>
+    <t>product_price_currency</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
     <t>product_price</t>
   </si>
   <si>
@@ -220,7 +226,13 @@
     <t>promo_id</t>
   </si>
   <si>
+    <t>current_price_currency</t>
+  </si>
+  <si>
     <t>current_price</t>
+  </si>
+  <si>
+    <t>promo_price_currency</t>
   </si>
   <si>
     <t>promo_price</t>
@@ -298,8 +310,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O69" totalsRowShown="0">
-  <autoFilter ref="A1:O69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O72" totalsRowShown="0">
+  <autoFilter ref="A1:O72"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Load Order"/>
     <tableColumn id="2" name="Table Name"/>
@@ -606,7 +618,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -614,7 +626,7 @@
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
@@ -1451,7 +1463,7 @@
         <v>17</v>
       </c>
       <c r="E23">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
         <v>26</v>
@@ -1714,14 +1726,14 @@
       <c r="C30" t="s">
         <v>45</v>
       </c>
-      <c r="D30">
-        <v>0</v>
+      <c r="D30" t="s">
+        <v>46</v>
       </c>
       <c r="E30">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F30" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="G30" t="s">
         <v>20</v>
@@ -1742,7 +1754,7 @@
         <v>20</v>
       </c>
       <c r="M30" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="O30" t="s">
         <v>24</v>
@@ -1756,37 +1768,37 @@
         <v>24</v>
       </c>
       <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31">
+        <v>19</v>
+      </c>
+      <c r="F31" t="s">
         <v>48</v>
       </c>
-      <c r="D31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31" t="s">
-        <v>18</v>
-      </c>
       <c r="G31" t="s">
         <v>20</v>
       </c>
       <c r="H31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K31" t="s">
         <v>20</v>
       </c>
       <c r="L31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M31" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="O31" t="s">
         <v>24</v>
@@ -1800,7 +1812,7 @@
         <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
@@ -1844,7 +1856,7 @@
         <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
         <v>17</v>
@@ -1853,25 +1865,25 @@
         <v>17</v>
       </c>
       <c r="F33" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="G33" t="s">
         <v>20</v>
       </c>
       <c r="H33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K33" t="s">
         <v>20</v>
       </c>
       <c r="L33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M33" t="s">
         <v>17</v>
@@ -1880,95 +1892,95 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
-      <c r="A35">
+    <row r="34" spans="1:15">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>53</v>
+      </c>
+      <c r="G34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" t="s">
+        <v>20</v>
+      </c>
+      <c r="K34" t="s">
+        <v>20</v>
+      </c>
+      <c r="L34" t="s">
+        <v>20</v>
+      </c>
+      <c r="M34" t="s">
+        <v>17</v>
+      </c>
+      <c r="O34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36">
         <v>2</v>
       </c>
-      <c r="B35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" t="s">
         <v>16</v>
       </c>
-      <c r="D35" t="s">
-        <v>17</v>
-      </c>
-      <c r="E35" t="s">
-        <v>17</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="D36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" t="s">
         <v>18</v>
       </c>
-      <c r="G35" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" t="s">
-        <v>20</v>
-      </c>
-      <c r="I35" t="s">
-        <v>19</v>
-      </c>
-      <c r="J35" t="s">
-        <v>20</v>
-      </c>
-      <c r="K35" t="s">
-        <v>20</v>
-      </c>
-      <c r="L35" t="s">
-        <v>20</v>
-      </c>
-      <c r="M35" t="s">
+      <c r="G36" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" t="s">
         <v>21</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N36" t="s">
         <v>22</v>
       </c>
-      <c r="O35" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15">
-      <c r="A36" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E36">
-        <v>80</v>
-      </c>
-      <c r="F36" t="s">
-        <v>26</v>
-      </c>
-      <c r="G36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" t="s">
-        <v>19</v>
-      </c>
-      <c r="J36" t="s">
-        <v>20</v>
-      </c>
-      <c r="K36" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" t="s">
-        <v>20</v>
-      </c>
-      <c r="M36" t="s">
-        <v>17</v>
-      </c>
       <c r="O36" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -1979,13 +1991,13 @@
         <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
       </c>
       <c r="E37">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="F37" t="s">
         <v>26</v>
@@ -2009,7 +2021,7 @@
         <v>20</v>
       </c>
       <c r="M37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="O37" t="s">
         <v>24</v>
@@ -2023,22 +2035,22 @@
         <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
       </c>
-      <c r="E38" t="s">
-        <v>17</v>
+      <c r="E38">
+        <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G38" t="s">
         <v>20</v>
       </c>
       <c r="H38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I38" t="s">
         <v>19</v>
@@ -2050,10 +2062,10 @@
         <v>20</v>
       </c>
       <c r="L38" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M38" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="O38" t="s">
         <v>24</v>
@@ -2067,7 +2079,7 @@
         <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D39" t="s">
         <v>17</v>
@@ -2076,13 +2088,13 @@
         <v>17</v>
       </c>
       <c r="F39" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="G39" t="s">
         <v>20</v>
       </c>
       <c r="H39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I39" t="s">
         <v>19</v>
@@ -2094,7 +2106,7 @@
         <v>20</v>
       </c>
       <c r="L39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M39" t="s">
         <v>17</v>
@@ -2103,62 +2115,59 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
-      <c r="A41">
+    <row r="40" spans="1:15">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" t="s">
+        <v>53</v>
+      </c>
+      <c r="G40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" t="s">
+        <v>20</v>
+      </c>
+      <c r="L40" t="s">
+        <v>20</v>
+      </c>
+      <c r="M40" t="s">
+        <v>17</v>
+      </c>
+      <c r="O40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="A42">
         <v>3</v>
       </c>
-      <c r="B41" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" t="s">
         <v>16</v>
-      </c>
-      <c r="D41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" t="s">
-        <v>17</v>
-      </c>
-      <c r="F41" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" t="s">
-        <v>19</v>
-      </c>
-      <c r="H41" t="s">
-        <v>20</v>
-      </c>
-      <c r="I41" t="s">
-        <v>19</v>
-      </c>
-      <c r="J41" t="s">
-        <v>20</v>
-      </c>
-      <c r="K41" t="s">
-        <v>20</v>
-      </c>
-      <c r="L41" t="s">
-        <v>20</v>
-      </c>
-      <c r="M41" t="s">
-        <v>21</v>
-      </c>
-      <c r="N41" t="s">
-        <v>22</v>
-      </c>
-      <c r="O41" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15">
-      <c r="A42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" t="s">
-        <v>59</v>
       </c>
       <c r="D42" t="s">
         <v>17</v>
@@ -2170,10 +2179,10 @@
         <v>18</v>
       </c>
       <c r="G42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H42" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I42" t="s">
         <v>19</v>
@@ -2185,13 +2194,16 @@
         <v>20</v>
       </c>
       <c r="L42" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M42" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="N42" t="s">
+        <v>22</v>
       </c>
       <c r="O42" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2202,7 +2214,7 @@
         <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D43" t="s">
         <v>17</v>
@@ -2246,7 +2258,7 @@
         <v>24</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
@@ -2255,13 +2267,13 @@
         <v>17</v>
       </c>
       <c r="F44" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="G44" t="s">
         <v>20</v>
       </c>
       <c r="H44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I44" t="s">
         <v>19</v>
@@ -2273,7 +2285,7 @@
         <v>20</v>
       </c>
       <c r="L44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M44" t="s">
         <v>17</v>
@@ -2282,62 +2294,59 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
-      <c r="A46">
+    <row r="45" spans="1:15">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" t="s">
+        <v>53</v>
+      </c>
+      <c r="G45" t="s">
+        <v>20</v>
+      </c>
+      <c r="H45" t="s">
+        <v>20</v>
+      </c>
+      <c r="I45" t="s">
+        <v>19</v>
+      </c>
+      <c r="J45" t="s">
+        <v>20</v>
+      </c>
+      <c r="K45" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45" t="s">
+        <v>20</v>
+      </c>
+      <c r="M45" t="s">
+        <v>17</v>
+      </c>
+      <c r="O45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="A47">
         <v>3</v>
       </c>
-      <c r="B46" t="s">
-        <v>61</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" t="s">
         <v>16</v>
-      </c>
-      <c r="D46" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" t="s">
-        <v>17</v>
-      </c>
-      <c r="F46" t="s">
-        <v>18</v>
-      </c>
-      <c r="G46" t="s">
-        <v>19</v>
-      </c>
-      <c r="H46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I46" t="s">
-        <v>19</v>
-      </c>
-      <c r="J46" t="s">
-        <v>20</v>
-      </c>
-      <c r="K46" t="s">
-        <v>20</v>
-      </c>
-      <c r="L46" t="s">
-        <v>20</v>
-      </c>
-      <c r="M46" t="s">
-        <v>21</v>
-      </c>
-      <c r="N46" t="s">
-        <v>22</v>
-      </c>
-      <c r="O46" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15">
-      <c r="A47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" t="s">
-        <v>24</v>
-      </c>
-      <c r="C47" t="s">
-        <v>59</v>
       </c>
       <c r="D47" t="s">
         <v>17</v>
@@ -2349,10 +2358,10 @@
         <v>18</v>
       </c>
       <c r="G47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H47" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I47" t="s">
         <v>19</v>
@@ -2364,13 +2373,16 @@
         <v>20</v>
       </c>
       <c r="L47" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M47" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="N47" t="s">
+        <v>22</v>
       </c>
       <c r="O47" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -2381,22 +2393,22 @@
         <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D48" t="s">
         <v>17</v>
       </c>
-      <c r="E48">
-        <v>200</v>
+      <c r="E48" t="s">
+        <v>17</v>
       </c>
       <c r="F48" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G48" t="s">
         <v>20</v>
       </c>
       <c r="H48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I48" t="s">
         <v>19</v>
@@ -2408,7 +2420,7 @@
         <v>20</v>
       </c>
       <c r="L48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M48" t="s">
         <v>17</v>
@@ -2425,7 +2437,7 @@
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D49" t="s">
         <v>17</v>
@@ -2443,10 +2455,10 @@
         <v>20</v>
       </c>
       <c r="I49" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J49" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K49" t="s">
         <v>20</v>
@@ -2461,62 +2473,59 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
-      <c r="A51">
+    <row r="50" spans="1:15">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50">
+        <v>200</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" t="s">
+        <v>20</v>
+      </c>
+      <c r="H50" t="s">
+        <v>20</v>
+      </c>
+      <c r="I50" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" t="s">
+        <v>19</v>
+      </c>
+      <c r="K50" t="s">
+        <v>20</v>
+      </c>
+      <c r="L50" t="s">
+        <v>20</v>
+      </c>
+      <c r="M50" t="s">
+        <v>17</v>
+      </c>
+      <c r="O50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52">
         <v>3</v>
       </c>
-      <c r="B51" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B52" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" t="s">
         <v>16</v>
-      </c>
-      <c r="D51" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" t="s">
-        <v>17</v>
-      </c>
-      <c r="F51" t="s">
-        <v>18</v>
-      </c>
-      <c r="G51" t="s">
-        <v>19</v>
-      </c>
-      <c r="H51" t="s">
-        <v>20</v>
-      </c>
-      <c r="I51" t="s">
-        <v>19</v>
-      </c>
-      <c r="J51" t="s">
-        <v>20</v>
-      </c>
-      <c r="K51" t="s">
-        <v>20</v>
-      </c>
-      <c r="L51" t="s">
-        <v>20</v>
-      </c>
-      <c r="M51" t="s">
-        <v>21</v>
-      </c>
-      <c r="N51" t="s">
-        <v>22</v>
-      </c>
-      <c r="O51" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15">
-      <c r="A52" t="s">
-        <v>24</v>
-      </c>
-      <c r="B52" t="s">
-        <v>24</v>
-      </c>
-      <c r="C52" t="s">
-        <v>59</v>
       </c>
       <c r="D52" t="s">
         <v>17</v>
@@ -2528,10 +2537,10 @@
         <v>18</v>
       </c>
       <c r="G52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H52" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I52" t="s">
         <v>19</v>
@@ -2543,13 +2552,16 @@
         <v>20</v>
       </c>
       <c r="L52" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M52" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="N52" t="s">
+        <v>22</v>
       </c>
       <c r="O52" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -2560,7 +2572,7 @@
         <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
@@ -2604,22 +2616,22 @@
         <v>24</v>
       </c>
       <c r="C54" t="s">
-        <v>68</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>19</v>
+        <v>69</v>
+      </c>
+      <c r="D54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" t="s">
+        <v>17</v>
       </c>
       <c r="F54" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="G54" t="s">
         <v>20</v>
       </c>
       <c r="H54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I54" t="s">
         <v>19</v>
@@ -2631,10 +2643,10 @@
         <v>20</v>
       </c>
       <c r="L54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M54" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="O54" t="s">
         <v>24</v>
@@ -2648,63 +2660,107 @@
         <v>24</v>
       </c>
       <c r="C55" t="s">
-        <v>69</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
+        <v>70</v>
+      </c>
+      <c r="D55" t="s">
+        <v>46</v>
       </c>
       <c r="E55">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="F55" t="s">
+        <v>26</v>
+      </c>
+      <c r="G55" t="s">
+        <v>20</v>
+      </c>
+      <c r="H55" t="s">
+        <v>20</v>
+      </c>
+      <c r="I55" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" t="s">
+        <v>20</v>
+      </c>
+      <c r="K55" t="s">
+        <v>20</v>
+      </c>
+      <c r="L55" t="s">
+        <v>20</v>
+      </c>
+      <c r="M55" t="s">
+        <v>17</v>
+      </c>
+      <c r="O55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" t="s">
+        <v>71</v>
+      </c>
+      <c r="D56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56">
+        <v>19</v>
+      </c>
+      <c r="F56" t="s">
+        <v>48</v>
+      </c>
+      <c r="G56" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56" t="s">
+        <v>20</v>
+      </c>
+      <c r="I56" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" t="s">
+        <v>20</v>
+      </c>
+      <c r="K56" t="s">
+        <v>20</v>
+      </c>
+      <c r="L56" t="s">
+        <v>20</v>
+      </c>
+      <c r="M56" t="s">
+        <v>49</v>
+      </c>
+      <c r="O56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" t="s">
         <v>46</v>
       </c>
-      <c r="G55" t="s">
-        <v>20</v>
-      </c>
-      <c r="H55" t="s">
-        <v>20</v>
-      </c>
-      <c r="I55" t="s">
-        <v>19</v>
-      </c>
-      <c r="J55" t="s">
-        <v>20</v>
-      </c>
-      <c r="K55" t="s">
-        <v>20</v>
-      </c>
-      <c r="L55" t="s">
-        <v>20</v>
-      </c>
-      <c r="M55" t="s">
-        <v>47</v>
-      </c>
-      <c r="O55" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15">
-      <c r="A57">
-        <v>2</v>
-      </c>
-      <c r="B57" t="s">
-        <v>70</v>
-      </c>
-      <c r="C57" t="s">
-        <v>16</v>
-      </c>
-      <c r="D57" t="s">
-        <v>17</v>
-      </c>
-      <c r="E57" t="s">
-        <v>17</v>
+      <c r="E57">
+        <v>3</v>
       </c>
       <c r="F57" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G57" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H57" t="s">
         <v>20</v>
@@ -2722,13 +2778,10 @@
         <v>20</v>
       </c>
       <c r="M57" t="s">
-        <v>21</v>
-      </c>
-      <c r="N57" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="O57" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:15">
@@ -2739,16 +2792,16 @@
         <v>24</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D58" t="s">
         <v>17</v>
       </c>
       <c r="E58">
-        <v>200</v>
+        <v>19</v>
       </c>
       <c r="F58" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="G58" t="s">
         <v>20</v>
@@ -2769,77 +2822,33 @@
         <v>20</v>
       </c>
       <c r="M58" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="O58" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
-      <c r="A59" t="s">
-        <v>24</v>
-      </c>
-      <c r="B59" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" t="s">
-        <v>17</v>
-      </c>
-      <c r="E59">
-        <v>200</v>
-      </c>
-      <c r="F59" t="s">
-        <v>26</v>
-      </c>
-      <c r="G59" t="s">
-        <v>20</v>
-      </c>
-      <c r="H59" t="s">
-        <v>20</v>
-      </c>
-      <c r="I59" t="s">
-        <v>19</v>
-      </c>
-      <c r="J59" t="s">
-        <v>20</v>
-      </c>
-      <c r="K59" t="s">
-        <v>20</v>
-      </c>
-      <c r="L59" t="s">
-        <v>20</v>
-      </c>
-      <c r="M59" t="s">
-        <v>17</v>
-      </c>
-      <c r="O59" t="s">
-        <v>24</v>
-      </c>
-    </row>
     <row r="60" spans="1:15">
-      <c r="A60" t="s">
-        <v>24</v>
+      <c r="A60">
+        <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="C60" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="D60" t="s">
         <v>17</v>
       </c>
-      <c r="E60">
-        <v>254</v>
+      <c r="E60" t="s">
+        <v>17</v>
       </c>
       <c r="F60" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H60" t="s">
         <v>20</v>
@@ -2857,10 +2866,13 @@
         <v>20</v>
       </c>
       <c r="M60" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="N60" t="s">
+        <v>22</v>
       </c>
       <c r="O60" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:15">
@@ -2871,16 +2883,16 @@
         <v>24</v>
       </c>
       <c r="C61" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="D61" t="s">
         <v>17</v>
       </c>
-      <c r="E61" t="s">
-        <v>17</v>
+      <c r="E61">
+        <v>200</v>
       </c>
       <c r="F61" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="G61" t="s">
         <v>20</v>
@@ -2915,22 +2927,22 @@
         <v>24</v>
       </c>
       <c r="C62" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
       </c>
-      <c r="E62" t="s">
-        <v>17</v>
+      <c r="E62">
+        <v>200</v>
       </c>
       <c r="F62" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G62" t="s">
         <v>20</v>
       </c>
       <c r="H62" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I62" t="s">
         <v>19</v>
@@ -2942,7 +2954,7 @@
         <v>20</v>
       </c>
       <c r="L62" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M62" t="s">
         <v>17</v>
@@ -2951,15 +2963,59 @@
         <v>24</v>
       </c>
     </row>
+    <row r="63" spans="1:15">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63">
+        <v>254</v>
+      </c>
+      <c r="F63" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" t="s">
+        <v>20</v>
+      </c>
+      <c r="H63" t="s">
+        <v>20</v>
+      </c>
+      <c r="I63" t="s">
+        <v>19</v>
+      </c>
+      <c r="J63" t="s">
+        <v>20</v>
+      </c>
+      <c r="K63" t="s">
+        <v>20</v>
+      </c>
+      <c r="L63" t="s">
+        <v>20</v>
+      </c>
+      <c r="M63" t="s">
+        <v>17</v>
+      </c>
+      <c r="O63" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="64" spans="1:15">
-      <c r="A64">
-        <v>4</v>
+      <c r="A64" t="s">
+        <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="C64" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="D64" t="s">
         <v>17</v>
@@ -2968,10 +3024,10 @@
         <v>17</v>
       </c>
       <c r="F64" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G64" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H64" t="s">
         <v>20</v>
@@ -2989,13 +3045,10 @@
         <v>20</v>
       </c>
       <c r="M64" t="s">
-        <v>21</v>
-      </c>
-      <c r="N64" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="O64" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:15">
@@ -3006,7 +3059,7 @@
         <v>24</v>
       </c>
       <c r="C65" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D65" t="s">
         <v>17</v>
@@ -3042,71 +3095,27 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
-      <c r="A66" t="s">
-        <v>24</v>
-      </c>
-      <c r="B66" t="s">
-        <v>24</v>
-      </c>
-      <c r="C66" t="s">
-        <v>67</v>
-      </c>
-      <c r="D66" t="s">
-        <v>17</v>
-      </c>
-      <c r="E66" t="s">
-        <v>17</v>
-      </c>
-      <c r="F66" t="s">
+    <row r="67" spans="1:15">
+      <c r="A67">
+        <v>4</v>
+      </c>
+      <c r="B67" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D67" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" t="s">
         <v>18</v>
       </c>
-      <c r="G66" t="s">
-        <v>20</v>
-      </c>
-      <c r="H66" t="s">
-        <v>19</v>
-      </c>
-      <c r="I66" t="s">
-        <v>19</v>
-      </c>
-      <c r="J66" t="s">
-        <v>20</v>
-      </c>
-      <c r="K66" t="s">
-        <v>20</v>
-      </c>
-      <c r="L66" t="s">
-        <v>19</v>
-      </c>
-      <c r="M66" t="s">
-        <v>17</v>
-      </c>
-      <c r="O66" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15">
-      <c r="A67" t="s">
-        <v>24</v>
-      </c>
-      <c r="B67" t="s">
-        <v>24</v>
-      </c>
-      <c r="C67" t="s">
-        <v>50</v>
-      </c>
-      <c r="D67" t="s">
-        <v>17</v>
-      </c>
-      <c r="E67" t="s">
-        <v>17</v>
-      </c>
-      <c r="F67" t="s">
-        <v>51</v>
-      </c>
       <c r="G67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H67" t="s">
         <v>20</v>
@@ -3124,9 +3133,144 @@
         <v>20</v>
       </c>
       <c r="M67" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="N67" t="s">
+        <v>22</v>
       </c>
       <c r="O67" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15">
+      <c r="A68" t="s">
+        <v>24</v>
+      </c>
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" t="s">
+        <v>82</v>
+      </c>
+      <c r="D68" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" t="s">
+        <v>18</v>
+      </c>
+      <c r="G68" t="s">
+        <v>20</v>
+      </c>
+      <c r="H68" t="s">
+        <v>19</v>
+      </c>
+      <c r="I68" t="s">
+        <v>19</v>
+      </c>
+      <c r="J68" t="s">
+        <v>20</v>
+      </c>
+      <c r="K68" t="s">
+        <v>20</v>
+      </c>
+      <c r="L68" t="s">
+        <v>19</v>
+      </c>
+      <c r="M68" t="s">
+        <v>17</v>
+      </c>
+      <c r="O68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
+      <c r="A69" t="s">
+        <v>24</v>
+      </c>
+      <c r="B69" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" t="s">
+        <v>69</v>
+      </c>
+      <c r="D69" t="s">
+        <v>17</v>
+      </c>
+      <c r="E69" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" t="s">
+        <v>20</v>
+      </c>
+      <c r="H69" t="s">
+        <v>19</v>
+      </c>
+      <c r="I69" t="s">
+        <v>19</v>
+      </c>
+      <c r="J69" t="s">
+        <v>20</v>
+      </c>
+      <c r="K69" t="s">
+        <v>20</v>
+      </c>
+      <c r="L69" t="s">
+        <v>19</v>
+      </c>
+      <c r="M69" t="s">
+        <v>17</v>
+      </c>
+      <c r="O69" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15">
+      <c r="A70" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" t="s">
+        <v>53</v>
+      </c>
+      <c r="G70" t="s">
+        <v>20</v>
+      </c>
+      <c r="H70" t="s">
+        <v>20</v>
+      </c>
+      <c r="I70" t="s">
+        <v>19</v>
+      </c>
+      <c r="J70" t="s">
+        <v>20</v>
+      </c>
+      <c r="K70" t="s">
+        <v>20</v>
+      </c>
+      <c r="L70" t="s">
+        <v>20</v>
+      </c>
+      <c r="M70" t="s">
+        <v>17</v>
+      </c>
+      <c r="O70" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Plural Names / Larger description Boxes
</commit_message>
<xml_diff>
--- a/Backend/group3site/jeans/generatedfiles/DataDict.xlsx
+++ b/Backend/group3site/jeans/generatedfiles/DataDict.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="81">
   <si>
     <t>Load Order</t>
   </si>
@@ -100,6 +100,9 @@
     <t>status_desc</t>
   </si>
   <si>
+    <t>max</t>
+  </si>
+  <si>
     <t>is_active</t>
   </si>
   <si>
@@ -151,12 +154,6 @@
     <t>product_desc</t>
   </si>
   <si>
-    <t>product_price_currency</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>product_price</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
     <t>promo_status_id</t>
   </si>
   <si>
+    <t>promo_desc</t>
+  </si>
+  <si>
     <t>ProductProductTag</t>
   </si>
   <si>
@@ -226,13 +226,7 @@
     <t>promo_id</t>
   </si>
   <si>
-    <t>current_price_currency</t>
-  </si>
-  <si>
     <t>current_price</t>
-  </si>
-  <si>
-    <t>promo_price_currency</t>
   </si>
   <si>
     <t>promo_price</t>
@@ -310,8 +304,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O72" totalsRowShown="0">
-  <autoFilter ref="A1:O72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O70" totalsRowShown="0">
+  <autoFilter ref="A1:O70"/>
   <tableColumns count="15">
     <tableColumn id="1" name="Load Order"/>
     <tableColumn id="2" name="Table Name"/>
@@ -618,7 +612,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -626,7 +620,7 @@
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
@@ -790,8 +784,8 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E4">
-        <v>200</v>
+      <c r="E4" t="s">
+        <v>28</v>
       </c>
       <c r="F4" t="s">
         <v>26</v>
@@ -829,7 +823,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -838,7 +832,7 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
         <v>20</v>
@@ -870,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -909,7 +903,7 @@
         <v>22</v>
       </c>
       <c r="O7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -969,8 +963,8 @@
       <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="E9">
-        <v>200</v>
+      <c r="E9" t="s">
+        <v>28</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
@@ -1008,7 +1002,7 @@
         <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -1017,7 +1011,7 @@
         <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G10" t="s">
         <v>20</v>
@@ -1049,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
         <v>16</v>
@@ -1088,7 +1082,7 @@
         <v>22</v>
       </c>
       <c r="O12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1148,8 +1142,8 @@
       <c r="D14" t="s">
         <v>17</v>
       </c>
-      <c r="E14">
-        <v>200</v>
+      <c r="E14" t="s">
+        <v>28</v>
       </c>
       <c r="F14" t="s">
         <v>26</v>
@@ -1187,7 +1181,7 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -1196,7 +1190,7 @@
         <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s">
         <v>20</v>
@@ -1228,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -1267,7 +1261,7 @@
         <v>22</v>
       </c>
       <c r="O17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1327,8 +1321,8 @@
       <c r="D19" t="s">
         <v>17</v>
       </c>
-      <c r="E19">
-        <v>200</v>
+      <c r="E19" t="s">
+        <v>28</v>
       </c>
       <c r="F19" t="s">
         <v>26</v>
@@ -1366,7 +1360,7 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -1375,7 +1369,7 @@
         <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G20" t="s">
         <v>20</v>
@@ -1407,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -1446,7 +1440,7 @@
         <v>22</v>
       </c>
       <c r="O22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1457,7 +1451,7 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D23" t="s">
         <v>17</v>
@@ -1501,13 +1495,13 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
       </c>
-      <c r="E24">
-        <v>200</v>
+      <c r="E24" t="s">
+        <v>28</v>
       </c>
       <c r="F24" t="s">
         <v>26</v>
@@ -1545,7 +1539,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -1586,7 +1580,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
         <v>16</v>
@@ -1625,7 +1619,7 @@
         <v>22</v>
       </c>
       <c r="O27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -1636,7 +1630,7 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
@@ -1680,13 +1674,13 @@
         <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D29" t="s">
         <v>17</v>
       </c>
-      <c r="E29">
-        <v>200</v>
+      <c r="E29" t="s">
+        <v>28</v>
       </c>
       <c r="F29" t="s">
         <v>26</v>
@@ -1724,16 +1718,16 @@
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" t="s">
         <v>46</v>
       </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
       <c r="E30">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G30" t="s">
         <v>20</v>
@@ -1754,7 +1748,7 @@
         <v>20</v>
       </c>
       <c r="M30" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="O30" t="s">
         <v>24</v>
@@ -1768,37 +1762,37 @@
         <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
       </c>
-      <c r="E31">
-        <v>19</v>
+      <c r="E31" t="s">
+        <v>17</v>
       </c>
       <c r="F31" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="G31" t="s">
         <v>20</v>
       </c>
       <c r="H31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K31" t="s">
         <v>20</v>
       </c>
       <c r="L31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M31" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="O31" t="s">
         <v>24</v>
@@ -1865,98 +1859,101 @@
         <v>17</v>
       </c>
       <c r="F33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G33" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" t="s">
+        <v>20</v>
+      </c>
+      <c r="L33" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33" t="s">
+        <v>17</v>
+      </c>
+      <c r="O33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" t="s">
         <v>18</v>
       </c>
-      <c r="G33" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" t="s">
-        <v>19</v>
-      </c>
-      <c r="I33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" t="s">
-        <v>19</v>
-      </c>
-      <c r="K33" t="s">
-        <v>20</v>
-      </c>
-      <c r="L33" t="s">
-        <v>19</v>
-      </c>
-      <c r="M33" t="s">
-        <v>17</v>
-      </c>
-      <c r="O33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" t="s">
-        <v>19</v>
-      </c>
-      <c r="J34" t="s">
-        <v>20</v>
-      </c>
-      <c r="K34" t="s">
-        <v>20</v>
-      </c>
-      <c r="L34" t="s">
-        <v>20</v>
-      </c>
-      <c r="M34" t="s">
-        <v>17</v>
-      </c>
-      <c r="O34" t="s">
-        <v>24</v>
+      <c r="G35" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" t="s">
+        <v>21</v>
+      </c>
+      <c r="N35" t="s">
+        <v>22</v>
+      </c>
+      <c r="O35" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:15">
-      <c r="A36">
-        <v>2</v>
+      <c r="A36" t="s">
+        <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
         <v>17</v>
       </c>
-      <c r="E36" t="s">
-        <v>17</v>
+      <c r="E36">
+        <v>80</v>
       </c>
       <c r="F36" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G36" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H36" t="s">
         <v>20</v>
@@ -1974,13 +1971,10 @@
         <v>20</v>
       </c>
       <c r="M36" t="s">
-        <v>21</v>
-      </c>
-      <c r="N36" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="O36" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -1997,7 +1991,7 @@
         <v>17</v>
       </c>
       <c r="E37">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
         <v>26</v>
@@ -2021,7 +2015,7 @@
         <v>20</v>
       </c>
       <c r="M37" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="O37" t="s">
         <v>24</v>
@@ -2040,17 +2034,17 @@
       <c r="D38" t="s">
         <v>17</v>
       </c>
-      <c r="E38">
-        <v>10</v>
+      <c r="E38" t="s">
+        <v>17</v>
       </c>
       <c r="F38" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G38" t="s">
         <v>20</v>
       </c>
       <c r="H38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I38" t="s">
         <v>19</v>
@@ -2062,10 +2056,10 @@
         <v>20</v>
       </c>
       <c r="L38" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M38" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="O38" t="s">
         <v>24</v>
@@ -2079,7 +2073,7 @@
         <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D39" t="s">
         <v>17</v>
@@ -2088,13 +2082,13 @@
         <v>17</v>
       </c>
       <c r="F39" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="G39" t="s">
         <v>20</v>
       </c>
       <c r="H39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I39" t="s">
         <v>19</v>
@@ -2106,7 +2100,7 @@
         <v>20</v>
       </c>
       <c r="L39" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M39" t="s">
         <v>17</v>
@@ -2123,16 +2117,16 @@
         <v>24</v>
       </c>
       <c r="C40" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D40" t="s">
         <v>17</v>
       </c>
       <c r="E40" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F40" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="G40" t="s">
         <v>20</v>
@@ -2141,10 +2135,10 @@
         <v>20</v>
       </c>
       <c r="I40" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K40" t="s">
         <v>20</v>
@@ -2302,16 +2296,16 @@
         <v>24</v>
       </c>
       <c r="C45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" t="s">
         <v>52</v>
-      </c>
-      <c r="D45" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" t="s">
-        <v>17</v>
-      </c>
-      <c r="F45" t="s">
-        <v>53</v>
       </c>
       <c r="G45" t="s">
         <v>20</v>
@@ -2662,14 +2656,14 @@
       <c r="C55" t="s">
         <v>70</v>
       </c>
-      <c r="D55" t="s">
-        <v>46</v>
+      <c r="D55">
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F55" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="G55" t="s">
         <v>20</v>
@@ -2690,7 +2684,7 @@
         <v>20</v>
       </c>
       <c r="M55" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="O55" t="s">
         <v>24</v>
@@ -2706,149 +2700,152 @@
       <c r="C56" t="s">
         <v>71</v>
       </c>
-      <c r="D56" t="s">
-        <v>17</v>
+      <c r="D56">
+        <v>0</v>
       </c>
       <c r="E56">
         <v>19</v>
       </c>
       <c r="F56" t="s">
+        <v>47</v>
+      </c>
+      <c r="G56" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56" t="s">
+        <v>20</v>
+      </c>
+      <c r="I56" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" t="s">
+        <v>20</v>
+      </c>
+      <c r="K56" t="s">
+        <v>20</v>
+      </c>
+      <c r="L56" t="s">
+        <v>20</v>
+      </c>
+      <c r="M56" t="s">
         <v>48</v>
       </c>
-      <c r="G56" t="s">
-        <v>20</v>
-      </c>
-      <c r="H56" t="s">
-        <v>20</v>
-      </c>
-      <c r="I56" t="s">
-        <v>19</v>
-      </c>
-      <c r="J56" t="s">
-        <v>20</v>
-      </c>
-      <c r="K56" t="s">
-        <v>20</v>
-      </c>
-      <c r="L56" t="s">
-        <v>20</v>
-      </c>
-      <c r="M56" t="s">
-        <v>49</v>
-      </c>
       <c r="O56" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
-      <c r="A57" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" t="s">
+    <row r="58" spans="1:15">
+      <c r="A58">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
         <v>72</v>
       </c>
-      <c r="D57" t="s">
-        <v>46</v>
-      </c>
-      <c r="E57">
-        <v>3</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="C58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" t="s">
+        <v>17</v>
+      </c>
+      <c r="F58" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58" t="s">
+        <v>19</v>
+      </c>
+      <c r="H58" t="s">
+        <v>20</v>
+      </c>
+      <c r="I58" t="s">
+        <v>19</v>
+      </c>
+      <c r="J58" t="s">
+        <v>20</v>
+      </c>
+      <c r="K58" t="s">
+        <v>20</v>
+      </c>
+      <c r="L58" t="s">
+        <v>20</v>
+      </c>
+      <c r="M58" t="s">
+        <v>21</v>
+      </c>
+      <c r="N58" t="s">
+        <v>22</v>
+      </c>
+      <c r="O58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59">
+        <v>200</v>
+      </c>
+      <c r="F59" t="s">
         <v>26</v>
       </c>
-      <c r="G57" t="s">
-        <v>20</v>
-      </c>
-      <c r="H57" t="s">
-        <v>20</v>
-      </c>
-      <c r="I57" t="s">
-        <v>19</v>
-      </c>
-      <c r="J57" t="s">
-        <v>20</v>
-      </c>
-      <c r="K57" t="s">
-        <v>20</v>
-      </c>
-      <c r="L57" t="s">
-        <v>20</v>
-      </c>
-      <c r="M57" t="s">
-        <v>17</v>
-      </c>
-      <c r="O57" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15">
-      <c r="A58" t="s">
-        <v>24</v>
-      </c>
-      <c r="B58" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" t="s">
-        <v>17</v>
-      </c>
-      <c r="E58">
-        <v>19</v>
-      </c>
-      <c r="F58" t="s">
-        <v>48</v>
-      </c>
-      <c r="G58" t="s">
-        <v>20</v>
-      </c>
-      <c r="H58" t="s">
-        <v>20</v>
-      </c>
-      <c r="I58" t="s">
-        <v>19</v>
-      </c>
-      <c r="J58" t="s">
-        <v>20</v>
-      </c>
-      <c r="K58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L58" t="s">
-        <v>20</v>
-      </c>
-      <c r="M58" t="s">
-        <v>49</v>
-      </c>
-      <c r="O58" t="s">
+      <c r="G59" t="s">
+        <v>20</v>
+      </c>
+      <c r="H59" t="s">
+        <v>20</v>
+      </c>
+      <c r="I59" t="s">
+        <v>19</v>
+      </c>
+      <c r="J59" t="s">
+        <v>20</v>
+      </c>
+      <c r="K59" t="s">
+        <v>20</v>
+      </c>
+      <c r="L59" t="s">
+        <v>20</v>
+      </c>
+      <c r="M59" t="s">
+        <v>17</v>
+      </c>
+      <c r="O59" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60">
-        <v>2</v>
+      <c r="A60" t="s">
+        <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="C60" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
       <c r="D60" t="s">
         <v>17</v>
       </c>
-      <c r="E60" t="s">
-        <v>17</v>
+      <c r="E60">
+        <v>200</v>
       </c>
       <c r="F60" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G60" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H60" t="s">
         <v>20</v>
@@ -2866,13 +2863,10 @@
         <v>20</v>
       </c>
       <c r="M60" t="s">
-        <v>21</v>
-      </c>
-      <c r="N60" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="O60" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:15">
@@ -2889,7 +2883,7 @@
         <v>17</v>
       </c>
       <c r="E61">
-        <v>200</v>
+        <v>254</v>
       </c>
       <c r="F61" t="s">
         <v>26</v>
@@ -2927,16 +2921,16 @@
         <v>24</v>
       </c>
       <c r="C62" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
       </c>
-      <c r="E62">
-        <v>200</v>
+      <c r="E62" t="s">
+        <v>17</v>
       </c>
       <c r="F62" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="G62" t="s">
         <v>20</v>
@@ -2971,95 +2965,51 @@
         <v>24</v>
       </c>
       <c r="C63" t="s">
+        <v>77</v>
+      </c>
+      <c r="D63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" t="s">
+        <v>18</v>
+      </c>
+      <c r="G63" t="s">
+        <v>20</v>
+      </c>
+      <c r="H63" t="s">
+        <v>19</v>
+      </c>
+      <c r="I63" t="s">
+        <v>19</v>
+      </c>
+      <c r="J63" t="s">
+        <v>20</v>
+      </c>
+      <c r="K63" t="s">
+        <v>20</v>
+      </c>
+      <c r="L63" t="s">
+        <v>19</v>
+      </c>
+      <c r="M63" t="s">
+        <v>17</v>
+      </c>
+      <c r="O63" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65" t="s">
         <v>78</v>
       </c>
-      <c r="D63" t="s">
-        <v>17</v>
-      </c>
-      <c r="E63">
-        <v>254</v>
-      </c>
-      <c r="F63" t="s">
-        <v>26</v>
-      </c>
-      <c r="G63" t="s">
-        <v>20</v>
-      </c>
-      <c r="H63" t="s">
-        <v>20</v>
-      </c>
-      <c r="I63" t="s">
-        <v>19</v>
-      </c>
-      <c r="J63" t="s">
-        <v>20</v>
-      </c>
-      <c r="K63" t="s">
-        <v>20</v>
-      </c>
-      <c r="L63" t="s">
-        <v>20</v>
-      </c>
-      <c r="M63" t="s">
-        <v>17</v>
-      </c>
-      <c r="O63" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15">
-      <c r="A64" t="s">
-        <v>24</v>
-      </c>
-      <c r="B64" t="s">
-        <v>24</v>
-      </c>
-      <c r="C64" t="s">
-        <v>52</v>
-      </c>
-      <c r="D64" t="s">
-        <v>17</v>
-      </c>
-      <c r="E64" t="s">
-        <v>17</v>
-      </c>
-      <c r="F64" t="s">
-        <v>53</v>
-      </c>
-      <c r="G64" t="s">
-        <v>20</v>
-      </c>
-      <c r="H64" t="s">
-        <v>20</v>
-      </c>
-      <c r="I64" t="s">
-        <v>19</v>
-      </c>
-      <c r="J64" t="s">
-        <v>20</v>
-      </c>
-      <c r="K64" t="s">
-        <v>20</v>
-      </c>
-      <c r="L64" t="s">
-        <v>20</v>
-      </c>
-      <c r="M64" t="s">
-        <v>17</v>
-      </c>
-      <c r="O64" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15">
-      <c r="A65" t="s">
-        <v>24</v>
-      </c>
-      <c r="B65" t="s">
-        <v>24</v>
-      </c>
       <c r="C65" t="s">
-        <v>79</v>
+        <v>16</v>
       </c>
       <c r="D65" t="s">
         <v>17</v>
@@ -3071,10 +3021,10 @@
         <v>18</v>
       </c>
       <c r="G65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H65" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I65" t="s">
         <v>19</v>
@@ -3086,24 +3036,71 @@
         <v>20</v>
       </c>
       <c r="L65" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M65" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="N65" t="s">
+        <v>22</v>
       </c>
       <c r="O65" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" t="s">
+        <v>80</v>
+      </c>
+      <c r="D66" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" t="s">
+        <v>20</v>
+      </c>
+      <c r="H66" t="s">
+        <v>19</v>
+      </c>
+      <c r="I66" t="s">
+        <v>19</v>
+      </c>
+      <c r="J66" t="s">
+        <v>20</v>
+      </c>
+      <c r="K66" t="s">
+        <v>20</v>
+      </c>
+      <c r="L66" t="s">
+        <v>19</v>
+      </c>
+      <c r="M66" t="s">
+        <v>17</v>
+      </c>
+      <c r="O66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:15">
-      <c r="A67">
-        <v>4</v>
+      <c r="A67" t="s">
+        <v>24</v>
       </c>
       <c r="B67" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="C67" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="D67" t="s">
         <v>17</v>
@@ -3115,10 +3112,10 @@
         <v>18</v>
       </c>
       <c r="G67" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I67" t="s">
         <v>19</v>
@@ -3130,16 +3127,13 @@
         <v>20</v>
       </c>
       <c r="L67" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M67" t="s">
-        <v>21</v>
-      </c>
-      <c r="N67" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="O67" t="s">
-        <v>81</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:15">
@@ -3150,7 +3144,7 @@
         <v>24</v>
       </c>
       <c r="C68" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D68" t="s">
         <v>17</v>
@@ -3159,13 +3153,13 @@
         <v>17</v>
       </c>
       <c r="F68" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="G68" t="s">
         <v>20</v>
       </c>
       <c r="H68" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I68" t="s">
         <v>19</v>
@@ -3177,100 +3171,12 @@
         <v>20</v>
       </c>
       <c r="L68" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M68" t="s">
         <v>17</v>
       </c>
       <c r="O68" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15">
-      <c r="A69" t="s">
-        <v>24</v>
-      </c>
-      <c r="B69" t="s">
-        <v>24</v>
-      </c>
-      <c r="C69" t="s">
-        <v>69</v>
-      </c>
-      <c r="D69" t="s">
-        <v>17</v>
-      </c>
-      <c r="E69" t="s">
-        <v>17</v>
-      </c>
-      <c r="F69" t="s">
-        <v>18</v>
-      </c>
-      <c r="G69" t="s">
-        <v>20</v>
-      </c>
-      <c r="H69" t="s">
-        <v>19</v>
-      </c>
-      <c r="I69" t="s">
-        <v>19</v>
-      </c>
-      <c r="J69" t="s">
-        <v>20</v>
-      </c>
-      <c r="K69" t="s">
-        <v>20</v>
-      </c>
-      <c r="L69" t="s">
-        <v>19</v>
-      </c>
-      <c r="M69" t="s">
-        <v>17</v>
-      </c>
-      <c r="O69" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15">
-      <c r="A70" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" t="s">
-        <v>24</v>
-      </c>
-      <c r="C70" t="s">
-        <v>52</v>
-      </c>
-      <c r="D70" t="s">
-        <v>17</v>
-      </c>
-      <c r="E70" t="s">
-        <v>17</v>
-      </c>
-      <c r="F70" t="s">
-        <v>53</v>
-      </c>
-      <c r="G70" t="s">
-        <v>20</v>
-      </c>
-      <c r="H70" t="s">
-        <v>20</v>
-      </c>
-      <c r="I70" t="s">
-        <v>19</v>
-      </c>
-      <c r="J70" t="s">
-        <v>20</v>
-      </c>
-      <c r="K70" t="s">
-        <v>20</v>
-      </c>
-      <c r="L70" t="s">
-        <v>20</v>
-      </c>
-      <c r="M70" t="s">
-        <v>17</v>
-      </c>
-      <c r="O70" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>